<commit_message>
[kbss-cvut/termit-ui#296] Internationalize Excel export.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/cs/export.xlsx
+++ b/src/main/resources/template/cs/export.xlsx
@@ -92,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -190,11 +191,11 @@
   </sheetPr>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="0" width="25.01"/>
   </cols>
@@ -270,11 +271,11 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="100.05"/>
@@ -291,7 +292,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[kbss-cvut/termit-ui#296] Increase definition column width.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/cs/export.xlsx
+++ b/src/main/resources/template/cs/export.xlsx
@@ -192,12 +192,14 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="6" style="0" width="25.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +277,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="100.05"/>

</xml_diff>